<commit_message>
Feb 21 from lab
</commit_message>
<xml_diff>
--- a/Figures/Figure3_compare_to_existing_supertype/previous_classification.xlsx
+++ b/Figures/Figure3_compare_to_existing_supertype/previous_classification.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10111"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ys0/workbench/HLA_clustering/Figures/Figure3_compare_to_existing_supertype/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADB425D3-8F44-D34D-B9AD-CCFC8ED750EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="17325" windowHeight="10890"/>
+    <workbookView xWindow="33480" yWindow="4580" windowWidth="17320" windowHeight="21480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -406,14 +412,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
-  <fonts count="21">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -427,152 +427,8 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="40">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -621,194 +477,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="9">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -816,251 +486,9 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1116,61 +544,17 @@
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
-    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
-    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
-    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
-    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
-    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
-    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
-    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
-    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
-    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
-    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
-    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
-    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
-    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
-    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
-    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
-    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
-    <cellStyle name="Bad" xfId="23" builtinId="27"/>
-    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
-    <cellStyle name="Total" xfId="25" builtinId="25"/>
-    <cellStyle name="Output" xfId="26" builtinId="21"/>
-    <cellStyle name="Currency" xfId="27" builtinId="4"/>
-    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
-    <cellStyle name="Note" xfId="29" builtinId="10"/>
-    <cellStyle name="Input" xfId="30" builtinId="20"/>
-    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
-    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
-    <cellStyle name="Good" xfId="33" builtinId="26"/>
-    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
-    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
-    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
-    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
-    <cellStyle name="Title" xfId="39" builtinId="15"/>
-    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
-    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
-    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
-    <cellStyle name="Comma" xfId="44" builtinId="3"/>
-    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
-    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
-    <cellStyle name="Percent" xfId="47" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1428,31 +812,31 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:I22"/>
+      <selection activeCell="J1" sqref="J1:J22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9" style="1"/>
-    <col min="2" max="2" width="9.2" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.3" customWidth="1"/>
-    <col min="4" max="4" width="5.9" style="2" customWidth="1"/>
+    <col min="2" max="2" width="9.1640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" customWidth="1"/>
+    <col min="4" max="4" width="5.83203125" style="2" customWidth="1"/>
     <col min="5" max="5" width="9" style="1"/>
     <col min="6" max="6" width="7.5" style="1" customWidth="1"/>
-    <col min="7" max="7" width="12.3" customWidth="1"/>
-    <col min="8" max="8" width="6.4" style="2" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" customWidth="1"/>
+    <col min="8" max="8" width="6.33203125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1478,7 +862,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -1506,7 +890,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>11</v>
       </c>
@@ -1534,7 +918,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>15</v>
       </c>
@@ -1562,7 +946,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>18</v>
       </c>
@@ -1590,12 +974,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>5</v>
@@ -1618,12 +1002,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>4</v>
+        <v>35</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>5</v>
@@ -1646,9 +1030,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>4</v>
@@ -1674,9 +1058,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>4</v>
@@ -1702,12 +1086,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>35</v>
+        <v>4</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>5</v>
@@ -1730,12 +1114,12 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>40</v>
+        <v>4</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>5</v>
@@ -1758,7 +1142,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
         <v>43</v>
       </c>
@@ -1786,7 +1170,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
         <v>47</v>
       </c>
@@ -1814,7 +1198,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
         <v>50</v>
       </c>
@@ -1842,7 +1226,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
         <v>53</v>
       </c>
@@ -1870,7 +1254,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="s">
         <v>56</v>
       </c>
@@ -1898,7 +1282,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="8" t="s">
         <v>59</v>
       </c>
@@ -1926,7 +1310,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="8" t="s">
         <v>62</v>
       </c>
@@ -1954,7 +1338,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="8" t="s">
         <v>65</v>
       </c>
@@ -1982,7 +1366,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="8" t="s">
         <v>69</v>
       </c>
@@ -2010,7 +1394,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="8" t="s">
         <v>72</v>
       </c>
@@ -2038,7 +1422,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="8" t="s">
         <v>76</v>
       </c>
@@ -2066,7 +1450,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="9" t="s">
         <v>79</v>
       </c>
@@ -2088,7 +1472,7 @@
       </c>
       <c r="H23" s="5"/>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" s="9" t="s">
         <v>82</v>
       </c>
@@ -2110,7 +1494,7 @@
       </c>
       <c r="H24" s="5"/>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" s="9" t="s">
         <v>84</v>
       </c>
@@ -2132,7 +1516,7 @@
       </c>
       <c r="H25" s="5"/>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" s="10" t="s">
         <v>86</v>
       </c>
@@ -2154,7 +1538,7 @@
       </c>
       <c r="H26" s="5"/>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" s="10" t="s">
         <v>88</v>
       </c>
@@ -2176,7 +1560,7 @@
       </c>
       <c r="H27" s="5"/>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" s="10" t="s">
         <v>90</v>
       </c>
@@ -2198,7 +1582,7 @@
       </c>
       <c r="H28" s="5"/>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" s="10" t="s">
         <v>92</v>
       </c>
@@ -2220,7 +1604,7 @@
       </c>
       <c r="H29" s="5"/>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" s="9" t="s">
         <v>94</v>
       </c>
@@ -2242,7 +1626,7 @@
       </c>
       <c r="H30" s="5"/>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" s="11" t="s">
         <v>96</v>
       </c>
@@ -2264,7 +1648,7 @@
       </c>
       <c r="H31" s="5"/>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" s="11" t="s">
         <v>99</v>
       </c>
@@ -2286,7 +1670,7 @@
       </c>
       <c r="H32" s="5"/>
     </row>
-    <row r="33" spans="5:8">
+    <row r="33" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E33" s="16" t="s">
         <v>101</v>
       </c>
@@ -2298,7 +1682,7 @@
       </c>
       <c r="H33" s="5"/>
     </row>
-    <row r="34" spans="5:8">
+    <row r="34" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E34" s="16" t="s">
         <v>102</v>
       </c>
@@ -2310,7 +1694,7 @@
       </c>
       <c r="H34" s="5"/>
     </row>
-    <row r="35" spans="5:8">
+    <row r="35" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E35" s="16" t="s">
         <v>103</v>
       </c>
@@ -2322,7 +1706,7 @@
       </c>
       <c r="H35" s="5"/>
     </row>
-    <row r="36" spans="5:8">
+    <row r="36" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E36" s="16" t="s">
         <v>104</v>
       </c>
@@ -2334,7 +1718,7 @@
       </c>
       <c r="H36" s="5"/>
     </row>
-    <row r="37" spans="5:8">
+    <row r="37" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E37" s="16" t="s">
         <v>105</v>
       </c>
@@ -2346,7 +1730,7 @@
       </c>
       <c r="H37" s="5"/>
     </row>
-    <row r="38" spans="5:8">
+    <row r="38" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E38" s="16" t="s">
         <v>106</v>
       </c>
@@ -2358,7 +1742,7 @@
       </c>
       <c r="H38" s="5"/>
     </row>
-    <row r="39" spans="5:8">
+    <row r="39" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E39" s="20" t="s">
         <v>107</v>
       </c>
@@ -2370,7 +1754,7 @@
       </c>
       <c r="H39" s="5"/>
     </row>
-    <row r="40" spans="5:8">
+    <row r="40" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E40" s="20" t="s">
         <v>108</v>
       </c>
@@ -2382,7 +1766,7 @@
       </c>
       <c r="H40" s="5"/>
     </row>
-    <row r="41" spans="5:8">
+    <row r="41" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E41" s="20" t="s">
         <v>109</v>
       </c>
@@ -2394,7 +1778,7 @@
       </c>
       <c r="H41" s="5"/>
     </row>
-    <row r="42" spans="5:8">
+    <row r="42" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E42" s="20" t="s">
         <v>110</v>
       </c>
@@ -2406,7 +1790,7 @@
       </c>
       <c r="H42" s="5"/>
     </row>
-    <row r="43" spans="5:8">
+    <row r="43" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E43" s="20" t="s">
         <v>111</v>
       </c>
@@ -2418,7 +1802,7 @@
       </c>
       <c r="H43" s="5"/>
     </row>
-    <row r="44" spans="5:8">
+    <row r="44" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E44" s="20" t="s">
         <v>112</v>
       </c>
@@ -2430,7 +1814,7 @@
       </c>
       <c r="H44" s="5"/>
     </row>
-    <row r="45" spans="5:8">
+    <row r="45" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E45" s="20" t="s">
         <v>113</v>
       </c>
@@ -2442,7 +1826,7 @@
       </c>
       <c r="H45" s="5"/>
     </row>
-    <row r="46" spans="5:8">
+    <row r="46" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E46" s="20" t="s">
         <v>114</v>
       </c>
@@ -2454,7 +1838,7 @@
       </c>
       <c r="H46" s="5"/>
     </row>
-    <row r="47" spans="5:8">
+    <row r="47" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E47" s="8" t="s">
         <v>115</v>
       </c>
@@ -2466,7 +1850,7 @@
       </c>
       <c r="H47" s="5"/>
     </row>
-    <row r="48" spans="5:8">
+    <row r="48" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E48" s="8" t="s">
         <v>117</v>
       </c>
@@ -2478,7 +1862,7 @@
       </c>
       <c r="H48" s="5"/>
     </row>
-    <row r="49" spans="5:8">
+    <row r="49" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E49" s="8" t="s">
         <v>118</v>
       </c>
@@ -2490,7 +1874,7 @@
       </c>
       <c r="H49" s="5"/>
     </row>
-    <row r="50" spans="5:8">
+    <row r="50" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E50" s="8" t="s">
         <v>119</v>
       </c>
@@ -2502,7 +1886,7 @@
       </c>
       <c r="H50" s="5"/>
     </row>
-    <row r="51" spans="5:8">
+    <row r="51" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E51" s="8" t="s">
         <v>120</v>
       </c>
@@ -2514,7 +1898,7 @@
       </c>
       <c r="H51" s="5"/>
     </row>
-    <row r="52" spans="5:8">
+    <row r="52" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E52" s="8" t="s">
         <v>121</v>
       </c>
@@ -2526,7 +1910,7 @@
       </c>
       <c r="H52" s="5"/>
     </row>
-    <row r="53" spans="5:8">
+    <row r="53" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E53" s="13" t="s">
         <v>122</v>
       </c>
@@ -2538,7 +1922,7 @@
       </c>
       <c r="H53" s="5"/>
     </row>
-    <row r="54" spans="5:8">
+    <row r="54" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E54" s="13" t="s">
         <v>124</v>
       </c>
@@ -2550,7 +1934,7 @@
       </c>
       <c r="H54" s="5"/>
     </row>
-    <row r="55" spans="5:8">
+    <row r="55" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E55" s="13" t="s">
         <v>125</v>
       </c>
@@ -2562,7 +1946,7 @@
       </c>
       <c r="H55" s="5"/>
     </row>
-    <row r="56" spans="5:8">
+    <row r="56" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E56" s="13" t="s">
         <v>126</v>
       </c>
@@ -2574,7 +1958,7 @@
       </c>
       <c r="H56" s="5"/>
     </row>
-    <row r="57" spans="5:8">
+    <row r="57" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E57" s="13" t="s">
         <v>127</v>
       </c>
@@ -2586,7 +1970,7 @@
       </c>
       <c r="H57" s="5"/>
     </row>
-    <row r="58" spans="5:8">
+    <row r="58" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E58" s="13" t="s">
         <v>128</v>
       </c>
@@ -2598,11 +1982,10 @@
       </c>
       <c r="H58" s="5"/>
     </row>
-    <row r="59" spans="5:5">
+    <row r="59" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E59" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>